<commit_message>
fazendo a analise manual mythril
</commit_message>
<xml_diff>
--- a/mythril/0.24.7_smartbugs-curated/manual_0.24.7_mythril_smartbugs-curatedresult_dasp.xlsx
+++ b/mythril/0.24.7_smartbugs-curated/manual_0.24.7_mythril_smartbugs-curatedresult_dasp.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="77">
   <si>
     <t>access_control</t>
   </si>
@@ -71,6 +71,9 @@
     <t>etherstore.sol.json</t>
   </si>
   <si>
+    <t>1  3</t>
+  </si>
+  <si>
     <t>FibonacciBalance.sol.json</t>
   </si>
   <si>
@@ -131,6 +134,9 @@
     <t>modifier_reentrancy.sol.json</t>
   </si>
   <si>
+    <t>1 4</t>
+  </si>
+  <si>
     <t>multiowned_vulnerable.sol.json</t>
   </si>
   <si>
@@ -164,7 +170,13 @@
     <t>reentrance.sol.json</t>
   </si>
   <si>
+    <t>1 2</t>
+  </si>
+  <si>
     <t>reentrancy_dao.sol.json</t>
+  </si>
+  <si>
+    <t>1 1</t>
   </si>
   <si>
     <t>reentrancy_simple.sol.json</t>
@@ -245,9 +257,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -276,40 +288,22 @@
       <charset val="1"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -323,7 +317,67 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -337,29 +391,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -373,33 +414,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -410,23 +428,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -483,7 +495,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="-0.5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -495,7 +507,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -507,13 +531,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -525,19 +555,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -549,7 +579,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -561,25 +645,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -591,79 +669,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -692,15 +704,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -712,39 +715,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -766,11 +736,53 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
       <bottom style="double">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -792,142 +804,142 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="12" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="32" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="28" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="12" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="12" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="12" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -946,6 +958,8 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="16" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="49">
@@ -1336,8 +1350,8 @@
   <sheetPr/>
   <dimension ref="A1:L64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54" defaultRowHeight="15"/>
@@ -1345,6 +1359,7 @@
     <col min="1" max="1" width="51.04" customWidth="1"/>
     <col min="2" max="2" width="16.5333333333333" customWidth="1"/>
     <col min="3" max="3" width="15.4333333333333" customWidth="1"/>
+    <col min="4" max="4" width="11" customWidth="1"/>
     <col min="5" max="5" width="8.5" customWidth="1"/>
     <col min="6" max="6" width="15.9" customWidth="1"/>
     <col min="7" max="7" width="13.3" customWidth="1"/>
@@ -1589,8 +1604,8 @@
       <c r="D7">
         <v>0</v>
       </c>
-      <c r="E7" s="5">
-        <v>4</v>
+      <c r="E7" s="12" t="s">
+        <v>17</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -1616,7 +1631,7 @@
     </row>
     <row r="8" ht="19.5" spans="1:12">
       <c r="A8" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -1654,7 +1669,7 @@
     </row>
     <row r="9" ht="19.5" spans="1:12">
       <c r="A9" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -1692,7 +1707,7 @@
     </row>
     <row r="10" ht="19.5" spans="1:12">
       <c r="A10" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B10" s="3">
         <v>1</v>
@@ -1730,7 +1745,7 @@
     </row>
     <row r="11" ht="19.5" spans="1:12">
       <c r="A11" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B11" s="4">
         <v>0</v>
@@ -1768,7 +1783,7 @@
     </row>
     <row r="12" ht="19.5" spans="1:12">
       <c r="A12" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B12" s="4">
         <v>0</v>
@@ -1806,7 +1821,7 @@
     </row>
     <row r="13" ht="19.5" spans="1:12">
       <c r="A13" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B13" s="4">
         <v>0</v>
@@ -1844,7 +1859,7 @@
     </row>
     <row r="14" ht="19.5" spans="1:12">
       <c r="A14" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -1882,7 +1897,7 @@
     </row>
     <row r="15" ht="19.5" spans="1:12">
       <c r="A15" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -1920,7 +1935,7 @@
     </row>
     <row r="16" ht="19.5" spans="1:12">
       <c r="A16" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -1958,7 +1973,7 @@
     </row>
     <row r="17" ht="19.5" spans="1:12">
       <c r="A17" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -1996,7 +2011,7 @@
     </row>
     <row r="18" ht="19.5" spans="1:12">
       <c r="A18" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B18">
         <v>0</v>
@@ -2034,7 +2049,7 @@
     </row>
     <row r="19" ht="19.5" spans="1:12">
       <c r="A19" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B19">
         <v>0</v>
@@ -2072,7 +2087,7 @@
     </row>
     <row r="20" ht="19.5" spans="1:12">
       <c r="A20" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B20">
         <v>0</v>
@@ -2110,7 +2125,7 @@
     </row>
     <row r="21" ht="19.5" spans="1:12">
       <c r="A21" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B21">
         <v>0</v>
@@ -2148,7 +2163,7 @@
     </row>
     <row r="22" ht="19.5" spans="1:12">
       <c r="A22" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B22">
         <v>0</v>
@@ -2186,7 +2201,7 @@
     </row>
     <row r="23" ht="19.5" spans="1:12">
       <c r="A23" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B23">
         <v>0</v>
@@ -2224,7 +2239,7 @@
     </row>
     <row r="24" ht="19.5" spans="1:12">
       <c r="A24" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B24">
         <v>0</v>
@@ -2262,7 +2277,7 @@
     </row>
     <row r="25" ht="19.5" spans="1:12">
       <c r="A25" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B25">
         <v>0</v>
@@ -2300,7 +2315,7 @@
     </row>
     <row r="26" ht="19.5" spans="1:12">
       <c r="A26" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B26" s="2">
         <v>1</v>
@@ -2338,7 +2353,7 @@
     </row>
     <row r="27" ht="19.5" spans="1:12">
       <c r="A27" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B27">
         <v>0</v>
@@ -2349,8 +2364,8 @@
       <c r="D27">
         <v>0</v>
       </c>
-      <c r="E27" s="5">
-        <v>5</v>
+      <c r="E27" s="13" t="s">
+        <v>38</v>
       </c>
       <c r="F27">
         <v>0</v>
@@ -2376,7 +2391,7 @@
     </row>
     <row r="28" ht="19.5" spans="1:12">
       <c r="A28" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B28" s="2">
         <v>1</v>
@@ -2414,7 +2429,7 @@
     </row>
     <row r="29" ht="19.5" spans="1:12">
       <c r="A29" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B29" s="2">
         <v>1</v>
@@ -2452,7 +2467,7 @@
     </row>
     <row r="30" ht="19.5" spans="1:12">
       <c r="A30" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B30">
         <v>0</v>
@@ -2490,7 +2505,7 @@
     </row>
     <row r="31" ht="19.5" spans="1:12">
       <c r="A31" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B31" s="3">
         <v>1</v>
@@ -2528,7 +2543,7 @@
     </row>
     <row r="32" ht="19.5" spans="1:12">
       <c r="A32" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B32">
         <v>0</v>
@@ -2566,7 +2581,7 @@
     </row>
     <row r="33" ht="19.5" spans="1:12">
       <c r="A33" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B33">
         <v>0</v>
@@ -2604,7 +2619,7 @@
     </row>
     <row r="34" spans="1:12">
       <c r="A34" s="7" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B34" s="4">
         <v>0</v>
@@ -2642,7 +2657,7 @@
     </row>
     <row r="35" spans="1:12">
       <c r="A35" s="7" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B35" s="4">
         <v>0</v>
@@ -2680,7 +2695,7 @@
     </row>
     <row r="36" ht="19.5" spans="1:12">
       <c r="A36" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B36" s="2">
         <v>2</v>
@@ -2718,7 +2733,7 @@
     </row>
     <row r="37" ht="19.5" spans="1:12">
       <c r="A37" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B37" s="4">
         <v>0</v>
@@ -2756,7 +2771,7 @@
     </row>
     <row r="38" ht="19.5" spans="1:12">
       <c r="A38" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B38" s="3">
         <v>1</v>
@@ -2767,8 +2782,8 @@
       <c r="D38">
         <v>0</v>
       </c>
-      <c r="E38" s="5">
-        <v>3</v>
+      <c r="E38" s="13" t="s">
+        <v>50</v>
       </c>
       <c r="F38" s="6">
         <v>1</v>
@@ -2794,7 +2809,7 @@
     </row>
     <row r="39" ht="19.5" spans="1:12">
       <c r="A39" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B39">
         <v>0</v>
@@ -2805,8 +2820,8 @@
       <c r="D39">
         <v>0</v>
       </c>
-      <c r="E39" s="5">
-        <v>2</v>
+      <c r="E39" s="13" t="s">
+        <v>52</v>
       </c>
       <c r="F39">
         <v>0</v>
@@ -2832,7 +2847,7 @@
     </row>
     <row r="40" ht="19.5" spans="1:12">
       <c r="A40" s="1" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="B40">
         <v>0</v>
@@ -2843,8 +2858,8 @@
       <c r="D40">
         <v>0</v>
       </c>
-      <c r="E40" s="5">
-        <v>2</v>
+      <c r="E40" s="13" t="s">
+        <v>52</v>
       </c>
       <c r="F40">
         <v>0</v>
@@ -2870,7 +2885,7 @@
     </row>
     <row r="41" ht="19.5" spans="1:12">
       <c r="A41" s="1" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="B41" s="3">
         <v>1</v>
@@ -2908,7 +2923,7 @@
     </row>
     <row r="42" ht="19.5" spans="1:12">
       <c r="A42" s="1" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="B42" s="4">
         <v>0</v>
@@ -2946,7 +2961,7 @@
     </row>
     <row r="43" ht="19.5" spans="1:12">
       <c r="A43" s="1" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="B43">
         <v>0</v>
@@ -2984,7 +2999,7 @@
     </row>
     <row r="44" ht="19.5" spans="1:12">
       <c r="A44" s="1" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="B44" s="3">
         <v>1</v>
@@ -2995,8 +3010,8 @@
       <c r="D44">
         <v>0</v>
       </c>
-      <c r="E44" s="5">
-        <v>3</v>
+      <c r="E44" s="13" t="s">
+        <v>50</v>
       </c>
       <c r="F44" s="6">
         <v>1</v>
@@ -3022,7 +3037,7 @@
     </row>
     <row r="45" ht="19.5" spans="1:12">
       <c r="A45" s="1" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="B45" s="2">
         <v>1</v>
@@ -3060,7 +3075,7 @@
     </row>
     <row r="46" ht="19.5" spans="1:12">
       <c r="A46" s="1" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B46">
         <v>0</v>
@@ -3098,7 +3113,7 @@
     </row>
     <row r="47" ht="19.5" spans="1:12">
       <c r="A47" s="1" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B47">
         <v>0</v>
@@ -3136,7 +3151,7 @@
     </row>
     <row r="48" ht="19.5" spans="1:12">
       <c r="A48" s="1" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B48">
         <v>0</v>
@@ -3174,7 +3189,7 @@
     </row>
     <row r="49" ht="19.5" spans="1:12">
       <c r="A49" s="1" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="B49">
         <v>0</v>
@@ -3212,7 +3227,7 @@
     </row>
     <row r="50" ht="19.5" spans="1:12">
       <c r="A50" s="1" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B50">
         <v>0</v>
@@ -3250,7 +3265,7 @@
     </row>
     <row r="51" spans="1:12">
       <c r="A51" s="7" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B51" s="4">
         <v>0</v>
@@ -3288,7 +3303,7 @@
     </row>
     <row r="52" ht="19.5" spans="1:12">
       <c r="A52" s="1" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B52" s="4">
         <v>0</v>
@@ -3326,7 +3341,7 @@
     </row>
     <row r="53" ht="19.5" spans="1:12">
       <c r="A53" s="1" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="B53" s="4">
         <v>0</v>
@@ -3364,7 +3379,7 @@
     </row>
     <row r="54" ht="19.5" spans="1:12">
       <c r="A54" s="1" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="B54" s="2">
         <v>1</v>
@@ -3402,7 +3417,7 @@
     </row>
     <row r="55" spans="1:12">
       <c r="A55" s="9" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="B55">
         <v>0</v>
@@ -3440,7 +3455,7 @@
     </row>
     <row r="56" spans="1:12">
       <c r="A56" s="10" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="B56">
         <v>0</v>
@@ -3478,7 +3493,7 @@
     </row>
     <row r="57" spans="1:12">
       <c r="A57" s="10" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="B57">
         <v>0</v>
@@ -3516,7 +3531,7 @@
     </row>
     <row r="58" spans="1:12">
       <c r="A58" s="10" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="B58">
         <v>0</v>
@@ -3592,7 +3607,7 @@
     </row>
     <row r="60" spans="1:12">
       <c r="A60" s="10" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="B60">
         <v>0</v>
@@ -3630,7 +3645,7 @@
     </row>
     <row r="61" spans="1:12">
       <c r="A61" s="10" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="B61">
         <v>0</v>
@@ -3668,7 +3683,7 @@
     </row>
     <row r="62" spans="1:12">
       <c r="A62" s="10" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="B62">
         <v>0</v>
@@ -3688,7 +3703,7 @@
       <c r="G62">
         <v>0</v>
       </c>
-      <c r="H62" s="12">
+      <c r="H62" s="14">
         <v>0</v>
       </c>
       <c r="I62" s="11">
@@ -3706,7 +3721,7 @@
     </row>
     <row r="63" spans="1:12">
       <c r="A63" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="B63">
         <v>0</v>
@@ -3744,7 +3759,7 @@
     </row>
     <row r="64" spans="1:12">
       <c r="A64" s="10" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="B64">
         <v>0</v>

</xml_diff>